<commit_message>
added title to tc01
</commit_message>
<xml_diff>
--- a/back-end-tests/week-19-test-cases.xlsx
+++ b/back-end-tests/week-19-test-cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mjukvarutestare 2020\testautomation\assignment004\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mjukvarutestare 2020\testautomation\assignment004\auto-back-annabrundin-simonelentini\back-end-tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A3EF2E-5923-4409-8060-17BE3966A291}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90E5FFD-8BA9-4396-93D9-CD5554E5454C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{B7D05850-246E-4C21-82DE-9F039E532BF4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>TC ID</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>TC01</t>
+  </si>
+  <si>
+    <t>Login endpoint</t>
   </si>
 </sst>
 </file>
@@ -273,35 +276,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,6 +295,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,77 +636,77 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.08984375" style="17" customWidth="1"/>
-    <col min="2" max="2" width="43.54296875" style="18" customWidth="1"/>
-    <col min="3" max="4" width="43.6328125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="35" style="18" customWidth="1"/>
+    <col min="1" max="1" width="26.08984375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="43.54296875" style="10" customWidth="1"/>
+    <col min="3" max="4" width="43.6328125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="35" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -725,72 +728,72 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.08984375" style="17" customWidth="1"/>
-    <col min="2" max="2" width="43.54296875" style="18" customWidth="1"/>
-    <col min="3" max="4" width="43.6328125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="35" style="18" customWidth="1"/>
+    <col min="1" max="1" width="26.08984375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="43.54296875" style="10" customWidth="1"/>
+    <col min="3" max="4" width="43.6328125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="35" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
created the TC02 logout
</commit_message>
<xml_diff>
--- a/back-end-tests/week-19-test-cases.xlsx
+++ b/back-end-tests/week-19-test-cases.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mjukvarutestare 2020\testautomation\assignment004\auto-back-annabrundin-simonelentini\back-end-tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenti\Documents\Skola\Testautomation\inlämningsuppgift\04\auto-back-annabrundin-simonelentini\back-end-tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90E5FFD-8BA9-4396-93D9-CD5554E5454C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721530D0-8336-430B-9CA4-B14CE5AB0C97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{B7D05850-246E-4C21-82DE-9F039E532BF4}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B7D05850-246E-4C21-82DE-9F039E532BF4}"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="2" r:id="rId1"/>
-    <sheet name="base form" sheetId="1" r:id="rId2"/>
+    <sheet name="TC02" sheetId="4" r:id="rId2"/>
+    <sheet name="base form" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>TC ID</t>
   </si>
@@ -71,6 +72,12 @@
   </si>
   <si>
     <t>Login endpoint</t>
+  </si>
+  <si>
+    <t>Logout endpoint</t>
+  </si>
+  <si>
+    <t>TC02</t>
   </si>
 </sst>
 </file>
@@ -337,7 +344,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -635,20 +642,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2261DB2E-B6F1-429D-9AF4-F45DF9B7E11F}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.08984375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="43.54296875" style="10" customWidth="1"/>
-    <col min="3" max="4" width="43.6328125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="43.5546875" style="10" customWidth="1"/>
+    <col min="3" max="4" width="43.6640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="10" customWidth="1"/>
     <col min="6" max="6" width="35" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -660,7 +667,7 @@
       <c r="E1" s="11"/>
       <c r="F1" s="12"/>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -670,7 +677,7 @@
       <c r="E2" s="14"/>
       <c r="F2" s="15"/>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -680,7 +687,7 @@
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -700,7 +707,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -719,6 +726,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E607829-59E5-4FBF-AC38-AE48A35486F5}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="43.5546875" style="10" customWidth="1"/>
+    <col min="3" max="4" width="43.6640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="35" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF077B6-0056-4A7C-B286-9B3177E9C7D2}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -726,16 +818,16 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.08984375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="43.54296875" style="10" customWidth="1"/>
-    <col min="3" max="4" width="43.6328125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="43.5546875" style="10" customWidth="1"/>
+    <col min="3" max="4" width="43.6640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="10" customWidth="1"/>
     <col min="6" max="6" width="35" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -747,7 +839,7 @@
       <c r="E1" s="11"/>
       <c r="F1" s="12"/>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -757,7 +849,7 @@
       <c r="E2" s="14"/>
       <c r="F2" s="15"/>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -767,7 +859,7 @@
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -787,7 +879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>

</xml_diff>